<commit_message>
Fixed process ID for TICC-173
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v7.5.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v7.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\edec-codelists\work-in-progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B5E5DC-875F-4201-B26C-82F036FC1647}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6298D80-28DB-4F46-B535-93D24C588F93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="282">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -889,6 +889,9 @@
   </si>
   <si>
     <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_2.0#conformant#urn:xoev-de:kosit:extension:xrechnung_2.0::D16B</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:2017:poacc:selfbilling:01:1.0</t>
   </si>
 </sst>
 </file>
@@ -1434,8 +1437,8 @@
   <dimension ref="A1:K106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3791,7 +3794,7 @@
         <v>142</v>
       </c>
       <c r="K73" s="4" t="s">
-        <v>158</v>
+        <v>281</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3822,7 +3825,7 @@
         <v>142</v>
       </c>
       <c r="K74" s="4" t="s">
-        <v>158</v>
+        <v>281</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added DocType for TICC-177
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v7.5.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v7.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6298D80-28DB-4F46-B535-93D24C588F93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9867BD-DCD1-4077-806C-B6EF1CBAA828}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
@@ -26,12 +26,12 @@
     <definedName name="_ftnref3" localSheetId="0">'Document Type'!$A$3</definedName>
     <definedName name="_ftnref4" localSheetId="0">'Document Type'!$A$4</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="284">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -788,9 +788,6 @@
   </si>
   <si>
     <t>TICC-137</t>
-  </si>
-  <si>
-    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:order_only:3</t>
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Order-2::Order##urn:fdc:peppol.eu:poacc:trns:order:3:restrictive:urn:www.agid.gov.it:trns:ordine:3.1::2.1</t>
@@ -892,6 +889,18 @@
   </si>
   <si>
     <t>cenbii-procid-ubl::urn:fdc:peppol.eu:2017:poacc:selfbilling:01:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:order_only:3
+cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:ordering:3</t>
+  </si>
+  <si>
+    <t>TICC-137
+TICC-177</t>
+  </si>
+  <si>
+    <t>TICC-102
+TICC-173</t>
   </si>
 </sst>
 </file>
@@ -1437,8 +1446,8 @@
   <dimension ref="A1:K106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3784,7 +3793,7 @@
         <v>0</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>245</v>
+        <v>283</v>
       </c>
       <c r="H73" s="3" t="b">
         <f>FALSE</f>
@@ -3794,7 +3803,7 @@
         <v>142</v>
       </c>
       <c r="K73" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3815,7 +3824,7 @@
         <v>0</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>245</v>
+        <v>283</v>
       </c>
       <c r="H74" s="3" t="b">
         <f>FALSE</f>
@@ -3825,7 +3834,7 @@
         <v>142</v>
       </c>
       <c r="K74" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4053,7 +4062,7 @@
     </row>
     <row r="82" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>60</v>
@@ -4068,7 +4077,7 @@
         <v>1</v>
       </c>
       <c r="F82" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>243</v>
@@ -4092,17 +4101,17 @@
         <v>60</v>
       </c>
       <c r="C83" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D83" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="D83" s="9" t="s">
+      <c r="E83" s="3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G83" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="E83" s="3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="H83" s="3" t="b">
         <f>FALSE</f>
@@ -4247,7 +4256,7 @@
     </row>
     <row r="88" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>60</v>
@@ -4262,7 +4271,7 @@
         <v>1</v>
       </c>
       <c r="F88" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G88" s="3" t="s">
         <v>241</v>
@@ -4280,7 +4289,7 @@
     </row>
     <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>60</v>
@@ -4295,7 +4304,7 @@
         <v>1</v>
       </c>
       <c r="F89" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G89" s="3" t="s">
         <v>241</v>
@@ -4313,7 +4322,7 @@
     </row>
     <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>60</v>
@@ -4328,7 +4337,7 @@
         <v>1</v>
       </c>
       <c r="F90" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G90" s="3" t="s">
         <v>241</v>
@@ -4346,7 +4355,7 @@
     </row>
     <row r="91" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>60</v>
@@ -4361,7 +4370,7 @@
         <v>1</v>
       </c>
       <c r="F91" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G91" s="3" t="s">
         <v>241</v>
@@ -4534,7 +4543,7 @@
     </row>
     <row r="97" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>60</v>
@@ -4549,7 +4558,7 @@
         <v>1</v>
       </c>
       <c r="F97" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>239</v>
@@ -4573,17 +4582,17 @@
         <v>60</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D98" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="E98" s="3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G98" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="E98" s="3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G98" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="H98" s="3" t="b">
         <f>FALSE</f>
@@ -4598,13 +4607,13 @@
     </row>
     <row r="99" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D99" s="9" t="s">
         <v>236</v>
@@ -4614,7 +4623,7 @@
         <v>0</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>250</v>
+        <v>282</v>
       </c>
       <c r="H99" s="3" t="b">
         <f>FALSE</f>
@@ -4623,19 +4632,19 @@
       <c r="J99" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="K99" s="4" t="s">
-        <v>251</v>
+      <c r="K99" s="3" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="100" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D100" s="9" t="s">
         <v>236</v>
@@ -4660,61 +4669,61 @@
     </row>
     <row r="101" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C101" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="B101" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C101" s="13" t="s">
+      <c r="D101" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="E101" s="3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G101" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="D101" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="E101" s="3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G101" s="3" t="s">
+      <c r="H101" s="3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="J101" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K101" s="15" t="s">
         <v>258</v>
-      </c>
-      <c r="H101" s="3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="J101" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="K101" s="15" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B102" s="14" t="s">
         <v>60</v>
       </c>
       <c r="C102" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="E102" s="3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G102" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="D102" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E102" s="3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G102" s="3" t="s">
+      <c r="H102" s="3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K102" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="H102" s="3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K102" s="3" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4725,17 +4734,17 @@
         <v>60</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E103" s="3" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H103" s="3" t="b">
         <f>FALSE</f>
@@ -4756,17 +4765,17 @@
         <v>60</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E104" s="3" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H104" s="3" t="b">
         <f>FALSE</f>
@@ -4787,17 +4796,17 @@
         <v>60</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E105" s="3" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H105" s="3" t="b">
         <f>FALSE</f>
@@ -4818,17 +4827,17 @@
         <v>60</v>
       </c>
       <c r="C106" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="E106" s="3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G106" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="D106" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="E106" s="3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G106" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="H106" s="3" t="b">
         <f>FALSE</f>

</xml_diff>